<commit_message>
Process Costing - Budgetary Control and Variance Analysis
</commit_message>
<xml_diff>
--- a/Management Accounting.xlsx
+++ b/Management Accounting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e12ce01b99ac21e8/GitHub/Investment Banking Technicals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1654" documentId="8_{F53C90D2-0365-4FFE-B83C-A64B747E4A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C42A7E2-4393-41A2-AA4A-7A71B064E526}"/>
+  <xr:revisionPtr revIDLastSave="2561" documentId="8_{F53C90D2-0365-4FFE-B83C-A64B747E4A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E32F7C0-2C5B-4B66-B972-B77AF8652DF9}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12660" windowHeight="16010" firstSheet="5" activeTab="7" xr2:uid="{61C2BC6E-EE60-412D-B102-A7A420EF0676}"/>
+    <workbookView xWindow="12390" yWindow="0" windowWidth="12660" windowHeight="16010" firstSheet="6" activeTab="12" xr2:uid="{61C2BC6E-EE60-412D-B102-A7A420EF0676}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <sheet name="7" sheetId="8" r:id="rId12"/>
     <sheet name="8" sheetId="9" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="603">
   <si>
     <t>300 glazed</t>
   </si>
@@ -1209,6 +1209,654 @@
   </si>
   <si>
     <t>In this scenario the extra day and two tickets are 1800 + 1800 + 450 + 200 = 4250 &lt; 5000 &lt; 6800 the alternative options. JP should take this option</t>
+  </si>
+  <si>
+    <t>end of May portable WIP</t>
+  </si>
+  <si>
+    <t>end of June portable WIP</t>
+  </si>
+  <si>
+    <t>Units completed in June</t>
+  </si>
+  <si>
+    <t>WIP by materials</t>
+  </si>
+  <si>
+    <t>WIP by conversion costs</t>
+  </si>
+  <si>
+    <t>materials cost in June</t>
+  </si>
+  <si>
+    <t>conversion cost in June</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>conversion cost</t>
+  </si>
+  <si>
+    <t>Step 1 track the physical flow</t>
+  </si>
+  <si>
+    <t>Beg inventory June 1</t>
+  </si>
+  <si>
+    <t>Started during June</t>
+  </si>
+  <si>
+    <t>Step 2 compute equivalent units</t>
+  </si>
+  <si>
+    <t>Units completed during June</t>
+  </si>
+  <si>
+    <t>Units in progress end of June</t>
+  </si>
+  <si>
+    <t>Total units accounted for</t>
+  </si>
+  <si>
+    <t>Step 3 collect costs to allocate</t>
+  </si>
+  <si>
+    <t>Costs incurred during June</t>
+  </si>
+  <si>
+    <t>Total costs to account for</t>
+  </si>
+  <si>
+    <t>Step 4 calculate the rate per unit</t>
+  </si>
+  <si>
+    <t>cost per unit</t>
+  </si>
+  <si>
+    <t>Step 5 allocate costs</t>
+  </si>
+  <si>
+    <t>Units completed in June COGM</t>
+  </si>
+  <si>
+    <t>Units in progress at eom end WIP</t>
+  </si>
+  <si>
+    <t>Total costs accounted for</t>
+  </si>
+  <si>
+    <t>EOM February WIP</t>
+  </si>
+  <si>
+    <t>EOM March WIP</t>
+  </si>
+  <si>
+    <t>units completed in March</t>
+  </si>
+  <si>
+    <t>WIP percent complete</t>
+  </si>
+  <si>
+    <t>Total manf costs March</t>
+  </si>
+  <si>
+    <t>units finished during March</t>
+  </si>
+  <si>
+    <t>equiv units complete total</t>
+  </si>
+  <si>
+    <t>equiv units complete WIP</t>
+  </si>
+  <si>
+    <t>cost of units finished in March</t>
+  </si>
+  <si>
+    <t>cost of units in WIP</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>material equiv units</t>
+  </si>
+  <si>
+    <t>coversion equiv units</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>Ending WIP inventory</t>
+  </si>
+  <si>
+    <t>Cost of good completed and transferred out</t>
+  </si>
+  <si>
+    <t>conversion starting at</t>
+  </si>
+  <si>
+    <t>EOM January WIP</t>
+  </si>
+  <si>
+    <t>Units completed February</t>
+  </si>
+  <si>
+    <t>WIP conversion costs</t>
+  </si>
+  <si>
+    <t>WIP material costs</t>
+  </si>
+  <si>
+    <t>metal</t>
+  </si>
+  <si>
+    <t>heating</t>
+  </si>
+  <si>
+    <t>conversion</t>
+  </si>
+  <si>
+    <t>packing</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>WIP equiv units</t>
+  </si>
+  <si>
+    <t>total equiv units</t>
+  </si>
+  <si>
+    <t>step 1</t>
+  </si>
+  <si>
+    <t>step 2</t>
+  </si>
+  <si>
+    <t>step 3 collect costs to allocate</t>
+  </si>
+  <si>
+    <t>step 4 calculate cost per equiv unit</t>
+  </si>
+  <si>
+    <t>COGM units completed during February</t>
+  </si>
+  <si>
+    <t>step 5 allocate costs</t>
+  </si>
+  <si>
+    <t>ending WIP</t>
+  </si>
+  <si>
+    <t>units started</t>
+  </si>
+  <si>
+    <t>costs added for year</t>
+  </si>
+  <si>
+    <t>units completed</t>
+  </si>
+  <si>
+    <t>ending finished goods inventory</t>
+  </si>
+  <si>
+    <t>beg finished goods inventory</t>
+  </si>
+  <si>
+    <t>beg WIP</t>
+  </si>
+  <si>
+    <t>beg WIP costs</t>
+  </si>
+  <si>
+    <t>end WIP # units</t>
+  </si>
+  <si>
+    <t>end WIP</t>
+  </si>
+  <si>
+    <t>beg WIP units</t>
+  </si>
+  <si>
+    <t>total equiv units wrt conversion</t>
+  </si>
+  <si>
+    <t>cost per equiv unit materials</t>
+  </si>
+  <si>
+    <t>current breakeven</t>
+  </si>
+  <si>
+    <t>new var costs</t>
+  </si>
+  <si>
+    <t>new breakeven</t>
+  </si>
+  <si>
+    <t>breakeven sales volume increase</t>
+  </si>
+  <si>
+    <t>estimated manf</t>
+  </si>
+  <si>
+    <t>desired profit</t>
+  </si>
+  <si>
+    <t>min price</t>
+  </si>
+  <si>
+    <t>breakeven volume annual</t>
+  </si>
+  <si>
+    <t>fixed costs monthly</t>
+  </si>
+  <si>
+    <t>EBT</t>
+  </si>
+  <si>
+    <t>annual volume</t>
+  </si>
+  <si>
+    <t>taxes paid</t>
+  </si>
+  <si>
+    <t>desired profit after taxes</t>
+  </si>
+  <si>
+    <t>volume required</t>
+  </si>
+  <si>
+    <t>var cost %</t>
+  </si>
+  <si>
+    <t>breakeven volume monthly</t>
+  </si>
+  <si>
+    <t>actual revenue</t>
+  </si>
+  <si>
+    <t>profit after taxes</t>
+  </si>
+  <si>
+    <t>desires profit monthly</t>
+  </si>
+  <si>
+    <t>required revenue</t>
+  </si>
+  <si>
+    <t>exp demand</t>
+  </si>
+  <si>
+    <t>price at max profit</t>
+  </si>
+  <si>
+    <t>monthly profit</t>
+  </si>
+  <si>
+    <t>contribution margin ratio</t>
+  </si>
+  <si>
+    <t>quantity sold</t>
+  </si>
+  <si>
+    <t>selling price per unit</t>
+  </si>
+  <si>
+    <t>var costs per unit</t>
+  </si>
+  <si>
+    <t>annual fixed costs</t>
+  </si>
+  <si>
+    <t>breakeven volume</t>
+  </si>
+  <si>
+    <t>2*b+m=150</t>
+  </si>
+  <si>
+    <t>desired rev</t>
+  </si>
+  <si>
+    <t>new volume</t>
+  </si>
+  <si>
+    <t>2*b+m=1150</t>
+  </si>
+  <si>
+    <t>assume b = m</t>
+  </si>
+  <si>
+    <t>new breakeven volume</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>used</t>
+  </si>
+  <si>
+    <t>breakeven volumes</t>
+  </si>
+  <si>
+    <t>0.5*n+0.6*u=840000</t>
+  </si>
+  <si>
+    <t>cleaning materials</t>
+  </si>
+  <si>
+    <t>var ov</t>
+  </si>
+  <si>
+    <t>fixed ov (3h at 5/h)</t>
+  </si>
+  <si>
+    <t>labor (3h at 15/h)</t>
+  </si>
+  <si>
+    <t>total cost</t>
+  </si>
+  <si>
+    <t>profit markup</t>
+  </si>
+  <si>
+    <t>their decision deals with excess demand</t>
+  </si>
+  <si>
+    <t>incremental cost</t>
+  </si>
+  <si>
+    <t>it might increase the total price by that amount to keep the same profit margin</t>
+  </si>
+  <si>
+    <t>units/month</t>
+  </si>
+  <si>
+    <t>framing var cost</t>
+  </si>
+  <si>
+    <t>new units sold</t>
+  </si>
+  <si>
+    <t>new sold</t>
+  </si>
+  <si>
+    <t>new framing var cost</t>
+  </si>
+  <si>
+    <t>excess supply</t>
+  </si>
+  <si>
+    <t>it would require extra  labor and materials but save $15/unt</t>
+  </si>
+  <si>
+    <t>total with</t>
+  </si>
+  <si>
+    <t>total without</t>
+  </si>
+  <si>
+    <t>total saved</t>
+  </si>
+  <si>
+    <t>new units produced</t>
+  </si>
+  <si>
+    <t>rev30outsource</t>
+  </si>
+  <si>
+    <t>rev15homemade</t>
+  </si>
+  <si>
+    <t>she should still outsource framing</t>
+  </si>
+  <si>
+    <t>monthly contribution margin</t>
+  </si>
+  <si>
+    <t>monthly volume</t>
+  </si>
+  <si>
+    <t>valves</t>
+  </si>
+  <si>
+    <t>maringal contribution</t>
+  </si>
+  <si>
+    <t>pumps lost</t>
+  </si>
+  <si>
+    <t>valves contribution</t>
+  </si>
+  <si>
+    <t>los contribution</t>
+  </si>
+  <si>
+    <t>net change in profit</t>
+  </si>
+  <si>
+    <t>breakeven unit contribution margin</t>
+  </si>
+  <si>
+    <t># customers</t>
+  </si>
+  <si>
+    <t>avg rev per visit</t>
+  </si>
+  <si>
+    <t>avg time per visit</t>
+  </si>
+  <si>
+    <t>small</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>large</t>
+  </si>
+  <si>
+    <t>monthly labor</t>
+  </si>
+  <si>
+    <t>l, m, then s revenue</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>s, m, then l revenue</t>
+  </si>
+  <si>
+    <t>customers</t>
+  </si>
+  <si>
+    <t>children</t>
+  </si>
+  <si>
+    <t>adults</t>
+  </si>
+  <si>
+    <t>ticket price</t>
+  </si>
+  <si>
+    <t>var cost per show</t>
+  </si>
+  <si>
+    <t>fixed cost per show</t>
+  </si>
+  <si>
+    <t>show</t>
+  </si>
+  <si>
+    <t>breakeven total rate</t>
+  </si>
+  <si>
+    <t>Randy should also consider the increased popularity of the reputation of the museum after sponsoring a school play</t>
+  </si>
+  <si>
+    <t>contribution margin per $1 wagered</t>
+  </si>
+  <si>
+    <t>replacement cost</t>
+  </si>
+  <si>
+    <t>replaced # machines</t>
+  </si>
+  <si>
+    <t>years until salvage</t>
+  </si>
+  <si>
+    <t>machine b increase wagered</t>
+  </si>
+  <si>
+    <t>cost each</t>
+  </si>
+  <si>
+    <t>today salvage val machine a</t>
+  </si>
+  <si>
+    <t>change in profit</t>
+  </si>
+  <si>
+    <t>No, the answer would remain the same because these are sunk costs</t>
+  </si>
+  <si>
+    <t>variance = actual value - budgeted (standard) value</t>
+  </si>
+  <si>
+    <t>flexible</t>
+  </si>
+  <si>
+    <t>as if</t>
+  </si>
+  <si>
+    <t>actual</t>
+  </si>
+  <si>
+    <t>tablets/bottle</t>
+  </si>
+  <si>
+    <t>mg/tablet</t>
+  </si>
+  <si>
+    <t>budgeted materials</t>
+  </si>
+  <si>
+    <t>budgeted price per mg</t>
+  </si>
+  <si>
+    <t>budgeted labor minutes</t>
+  </si>
+  <si>
+    <t>budgeted labor rate</t>
+  </si>
+  <si>
+    <t>actual product bottles produced</t>
+  </si>
+  <si>
+    <t>labor price variance</t>
+  </si>
+  <si>
+    <t>labor quantity variance</t>
+  </si>
+  <si>
+    <t>actual q of materials recent month</t>
+  </si>
+  <si>
+    <t>actual p paid for materials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">actual q labor used </t>
+  </si>
+  <si>
+    <t>actual p per hour</t>
+  </si>
+  <si>
+    <t>actual profit</t>
+  </si>
+  <si>
+    <t>fixed cost spending variance</t>
+  </si>
+  <si>
+    <t>total profit variance</t>
+  </si>
+  <si>
+    <t>variable cost variance</t>
+  </si>
+  <si>
+    <t>master budget profit</t>
+  </si>
+  <si>
+    <t>flexible budget profit</t>
+  </si>
+  <si>
+    <t>use equations from notes</t>
+  </si>
+  <si>
+    <t>beg balance (kg)</t>
+  </si>
+  <si>
+    <t>beg balance ($)</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>transaction</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>purchase</t>
+  </si>
+  <si>
+    <t>units (kg)</t>
+  </si>
+  <si>
+    <t>issued out</t>
+  </si>
+  <si>
+    <t>isued out</t>
+  </si>
+  <si>
+    <t>end balance (kg)</t>
+  </si>
+  <si>
+    <t>end balance ($)</t>
+  </si>
+  <si>
+    <t>cost of material issued out</t>
+  </si>
+  <si>
+    <t>purchase price variance</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>kgs</t>
+  </si>
+  <si>
+    <t>beg inventory</t>
+  </si>
+  <si>
+    <t>plus purchases</t>
+  </si>
+  <si>
+    <t>minus issued out</t>
+  </si>
+  <si>
+    <t>plus purchase price variance</t>
+  </si>
+  <si>
+    <t>ending inventory</t>
   </si>
 </sst>
 </file>
@@ -1250,11 +1898,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1270,6 +1919,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1846,17 +2499,681 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0571809C-0523-4EF0-AA09-490785578CBF}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="21" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>321</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>5.33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>459</v>
+      </c>
+      <c r="D8">
+        <f>D6/(D4-D5)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>460</v>
+      </c>
+      <c r="D9">
+        <f>D5*1.5</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>461</v>
+      </c>
+      <c r="D10">
+        <f>D6/(D4-D9)</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>462</v>
+      </c>
+      <c r="D12">
+        <f>D10-D8</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>463</v>
+      </c>
+      <c r="D14">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>464</v>
+      </c>
+      <c r="D15">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>465</v>
+      </c>
+      <c r="D16">
+        <f>(D15+D6)/D14+D5</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B18">
+        <v>5.38</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>467</v>
+      </c>
+      <c r="D21">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>437</v>
+      </c>
+      <c r="D22">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s">
+        <v>466</v>
+      </c>
+      <c r="D24">
+        <f>12*(D21/(D19-D20))</f>
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>469</v>
+      </c>
+      <c r="D26">
+        <v>750000</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>468</v>
+      </c>
+      <c r="D27">
+        <f>D26*(D19-D20)-12*D21</f>
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C28" t="s">
+        <v>470</v>
+      </c>
+      <c r="D28">
+        <f>D27*D22</f>
+        <v>37500</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C29" t="s">
+        <v>256</v>
+      </c>
+      <c r="D29">
+        <f>D27-D28</f>
+        <v>112500</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B31">
+        <v>5.39</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C32" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C33" t="s">
+        <v>107</v>
+      </c>
+      <c r="D33">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C34" t="s">
+        <v>467</v>
+      </c>
+      <c r="D34">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C35" t="s">
+        <v>437</v>
+      </c>
+      <c r="D35">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C36" t="s">
+        <v>471</v>
+      </c>
+      <c r="D36">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C38" t="s">
+        <v>472</v>
+      </c>
+      <c r="D38">
+        <f>(12*D34+D36/(1-D35))/(D32-D33)</f>
+        <v>760000</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B40">
+        <v>5.41</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C41" t="s">
+        <v>473</v>
+      </c>
+      <c r="D41">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C42" t="s">
+        <v>467</v>
+      </c>
+      <c r="D42">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C43" t="s">
+        <v>437</v>
+      </c>
+      <c r="D43">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
+        <v>474</v>
+      </c>
+      <c r="D45">
+        <f>D42/(1-D41)</f>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" t="s">
+        <v>475</v>
+      </c>
+      <c r="D47">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C48" t="s">
+        <v>364</v>
+      </c>
+      <c r="D48">
+        <f>D47*(1-D41)-D42</f>
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C49" t="s">
+        <v>476</v>
+      </c>
+      <c r="D49">
+        <f>D48*(1-D43)</f>
+        <v>13650</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B51" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" t="s">
+        <v>477</v>
+      </c>
+      <c r="D51">
+        <v>7280</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C52" t="s">
+        <v>478</v>
+      </c>
+      <c r="D52">
+        <f>(D51/(1-D43)+D42)/(1-D41)</f>
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B54">
+        <v>5.43</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C55" t="s">
+        <v>96</v>
+      </c>
+      <c r="D55" t="s">
+        <v>479</v>
+      </c>
+      <c r="E55" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C56">
+        <v>32.5</v>
+      </c>
+      <c r="D56">
+        <v>300</v>
+      </c>
+      <c r="E56">
+        <f>D56*(C56-D$62)-D63</f>
+        <v>4950</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C57">
+        <f>C56-2.5</f>
+        <v>30</v>
+      </c>
+      <c r="D57">
+        <f>D56+50</f>
+        <v>350</v>
+      </c>
+      <c r="E57">
+        <f t="shared" ref="E57:E60" si="0">D57*(C57-D$62)-D64</f>
+        <v>8400</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C58">
+        <f t="shared" ref="C58:C60" si="1">C57-2.5</f>
+        <v>27.5</v>
+      </c>
+      <c r="D58">
+        <f t="shared" ref="D58:D60" si="2">D57+50</f>
+        <v>400</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="0"/>
+        <v>8572.5</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C59">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="2"/>
+        <v>450</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="0"/>
+        <v>8550</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C60">
+        <f t="shared" si="1"/>
+        <v>22.5</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="E60" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C62" t="s">
+        <v>107</v>
+      </c>
+      <c r="D62">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C63" t="s">
+        <v>30</v>
+      </c>
+      <c r="D63">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C65" t="s">
+        <v>480</v>
+      </c>
+      <c r="D65">
+        <f>C58</f>
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B67">
+        <v>5.46</v>
+      </c>
+      <c r="D67" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C68" t="s">
+        <v>483</v>
+      </c>
+      <c r="D68">
+        <v>800</v>
+      </c>
+      <c r="E68">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C69" t="s">
+        <v>484</v>
+      </c>
+      <c r="D69">
+        <v>200</v>
+      </c>
+      <c r="E69">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C70" t="s">
+        <v>485</v>
+      </c>
+      <c r="D70">
+        <v>100</v>
+      </c>
+      <c r="E70">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C71" t="s">
+        <v>486</v>
+      </c>
+      <c r="D71">
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B73" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" t="s">
+        <v>487</v>
+      </c>
+      <c r="D73" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B75" t="s">
+        <v>9</v>
+      </c>
+      <c r="C75" t="s">
+        <v>489</v>
+      </c>
+      <c r="D75">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C76" t="s">
+        <v>490</v>
+      </c>
+      <c r="D76" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B78" t="s">
+        <v>11</v>
+      </c>
+      <c r="C78" t="s">
+        <v>492</v>
+      </c>
+      <c r="D78" t="s">
+        <v>9</v>
+      </c>
+      <c r="E78" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C79" t="s">
+        <v>493</v>
+      </c>
+      <c r="D79">
+        <v>50</v>
+      </c>
+      <c r="E79">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B81">
+        <v>5.48</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="D82" t="s">
+        <v>494</v>
+      </c>
+      <c r="E82" t="s">
+        <v>495</v>
+      </c>
+      <c r="F82" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C83" t="s">
+        <v>27</v>
+      </c>
+      <c r="D83">
+        <v>1500000</v>
+      </c>
+      <c r="E83">
+        <v>500000</v>
+      </c>
+      <c r="F83">
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C84" t="s">
+        <v>107</v>
+      </c>
+      <c r="D84">
+        <v>750000</v>
+      </c>
+      <c r="E84">
+        <v>200000</v>
+      </c>
+      <c r="F84">
+        <v>950000</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C85" t="s">
+        <v>337</v>
+      </c>
+      <c r="D85">
+        <v>750000</v>
+      </c>
+      <c r="E85">
+        <v>300000</v>
+      </c>
+      <c r="F85">
+        <v>1050000</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C86" t="s">
+        <v>30</v>
+      </c>
+      <c r="F86">
+        <v>840000</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C87" t="s">
+        <v>364</v>
+      </c>
+      <c r="F87">
+        <v>210000</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B89" t="s">
+        <v>7</v>
+      </c>
+      <c r="C89" t="s">
+        <v>496</v>
+      </c>
+      <c r="D89" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C90" t="s">
+        <v>482</v>
+      </c>
+      <c r="D90">
+        <f>D85/D83</f>
+        <v>0.5</v>
+      </c>
+      <c r="E90">
+        <f>E85/E83</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B92" t="s">
+        <v>9</v>
+      </c>
+      <c r="C92" t="s">
+        <v>464</v>
+      </c>
+      <c r="D92">
+        <v>1050000</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C93" t="s">
+        <v>478</v>
+      </c>
+      <c r="D93">
+        <f>D92+F86</f>
+        <v>1890000</v>
       </c>
     </row>
   </sheetData>
@@ -1866,17 +3183,823 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0832F0C9-E4F9-4241-BBD3-E7588556F34F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="17.26953125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>322</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>6.32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>498</v>
+      </c>
+      <c r="D4">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>501</v>
+      </c>
+      <c r="D5">
+        <v>45</v>
+      </c>
+      <c r="E5">
+        <f>D5/3</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>499</v>
+      </c>
+      <c r="D6">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>500</v>
+      </c>
+      <c r="D7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>502</v>
+      </c>
+      <c r="D8">
+        <f>D7+D6+D5+D4</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>503</v>
+      </c>
+      <c r="D9">
+        <f>D8*0.5</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10">
+        <f>D9+D8</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>248</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C13">
+        <f>3*D13*D12+3*E13*E12</f>
+        <v>54</v>
+      </c>
+      <c r="D13">
+        <v>15</v>
+      </c>
+      <c r="E13">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C14">
+        <f>C13*150</f>
+        <v>8100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>505</v>
+      </c>
+      <c r="D17">
+        <f>D4+C13+D6+D7</f>
+        <v>89</v>
+      </c>
+      <c r="E17">
+        <f>D17*150</f>
+        <v>13350</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B21">
+        <v>6.34</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>507</v>
+      </c>
+      <c r="D22">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
+        <v>225</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>467</v>
+      </c>
+      <c r="D25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
+        <v>508</v>
+      </c>
+      <c r="D26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C28" t="s">
+        <v>509</v>
+      </c>
+      <c r="D28">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C29" t="s">
+        <v>510</v>
+      </c>
+      <c r="D29">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C31" t="s">
+        <v>511</v>
+      </c>
+      <c r="D31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C36" t="s">
+        <v>514</v>
+      </c>
+      <c r="D36">
+        <f>D29*D31</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C37" t="s">
+        <v>515</v>
+      </c>
+      <c r="D37">
+        <f>D26*D29</f>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C38" t="s">
+        <v>516</v>
+      </c>
+      <c r="D38">
+        <f>D37-D36</f>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" t="s">
+        <v>517</v>
+      </c>
+      <c r="D40">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C41" t="s">
+        <v>514</v>
+      </c>
+      <c r="D41">
+        <f>D40*D31</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C42" t="s">
+        <v>515</v>
+      </c>
+      <c r="D42">
+        <f>D40*D26</f>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C44" t="s">
+        <v>518</v>
+      </c>
+      <c r="D44">
+        <f>D29*(D23-D24-D26)-D25</f>
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C45" t="s">
+        <v>519</v>
+      </c>
+      <c r="D45">
+        <f>D40*(D23-D24-D31)-D25</f>
+        <v>605</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C47" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B49">
+        <v>6.44</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C50" t="s">
+        <v>521</v>
+      </c>
+      <c r="D50">
+        <v>125000</v>
+      </c>
+      <c r="E50">
+        <f>D50*E53/D53</f>
+        <v>106250</v>
+      </c>
+      <c r="F50">
+        <f>D50-E50</f>
+        <v>18750</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C51" t="s">
+        <v>481</v>
+      </c>
+      <c r="D51">
+        <v>50000</v>
+      </c>
+      <c r="E51">
+        <f>D51*E53/D53</f>
+        <v>42500</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C52" t="s">
+        <v>522</v>
+      </c>
+      <c r="D52">
+        <v>2500</v>
+      </c>
+      <c r="E52">
+        <f>D52*E53/D53</f>
+        <v>2125</v>
+      </c>
+      <c r="G52">
+        <f>D53/D52</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C53" t="s">
+        <v>149</v>
+      </c>
+      <c r="D53">
+        <v>10000</v>
+      </c>
+      <c r="E53">
+        <f>D53-E57</f>
+        <v>8500</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C55" t="s">
+        <v>523</v>
+      </c>
+      <c r="D55">
+        <v>500</v>
+      </c>
+      <c r="H55" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C56" t="s">
+        <v>524</v>
+      </c>
+      <c r="D56">
+        <v>30</v>
+      </c>
+      <c r="H56">
+        <f>E57/G52</f>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C57" t="s">
+        <v>149</v>
+      </c>
+      <c r="D57">
+        <v>3</v>
+      </c>
+      <c r="E57">
+        <f>D57*D55</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" t="s">
+        <v>526</v>
+      </c>
+      <c r="D59">
+        <f>D55*D56</f>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C60" t="s">
+        <v>527</v>
+      </c>
+      <c r="D60">
+        <f>F50</f>
+        <v>18750</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C61" t="s">
+        <v>528</v>
+      </c>
+      <c r="D61">
+        <f>D59-D60</f>
+        <v>-3750</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" t="s">
+        <v>529</v>
+      </c>
+      <c r="D63">
+        <f>D60/D55</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B65">
+        <v>6.45</v>
+      </c>
+      <c r="D65" t="s">
+        <v>533</v>
+      </c>
+      <c r="E65" t="s">
+        <v>534</v>
+      </c>
+      <c r="F65" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C66" t="s">
+        <v>530</v>
+      </c>
+      <c r="D66">
+        <v>50</v>
+      </c>
+      <c r="E66">
+        <v>25</v>
+      </c>
+      <c r="F66">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C67" t="s">
+        <v>531</v>
+      </c>
+      <c r="D67">
+        <v>15000</v>
+      </c>
+      <c r="E67">
+        <v>30000</v>
+      </c>
+      <c r="F67">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C68" t="s">
+        <v>532</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>2</v>
+      </c>
+      <c r="F68">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C70" t="s">
+        <v>536</v>
+      </c>
+      <c r="D70">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B72" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72" t="s">
+        <v>538</v>
+      </c>
+      <c r="D72">
+        <f>D70</f>
+        <v>125</v>
+      </c>
+      <c r="E72">
+        <f>D72-F68*F66</f>
+        <v>75</v>
+      </c>
+      <c r="F72">
+        <f>F67*F66</f>
+        <v>450000</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C73" t="s">
+        <v>85</v>
+      </c>
+      <c r="D73">
+        <f>E72</f>
+        <v>75</v>
+      </c>
+      <c r="E73">
+        <f>D73-E68*E66</f>
+        <v>25</v>
+      </c>
+      <c r="F73">
+        <f>E66*E67</f>
+        <v>750000</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C74" t="s">
+        <v>539</v>
+      </c>
+      <c r="D74">
+        <f>E73</f>
+        <v>25</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <f>D74*D67</f>
+        <v>375000</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F75">
+        <f>F74+F73+F72</f>
+        <v>1575000</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C76" t="s">
+        <v>537</v>
+      </c>
+      <c r="D76">
+        <f>F75</f>
+        <v>1575000</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B78" t="s">
+        <v>9</v>
+      </c>
+      <c r="C78" t="s">
+        <v>539</v>
+      </c>
+      <c r="D78">
+        <v>125</v>
+      </c>
+      <c r="E78">
+        <f>D78-D68*D66</f>
+        <v>75</v>
+      </c>
+      <c r="F78">
+        <f>(D78-E78)*D67</f>
+        <v>750000</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C79" t="s">
+        <v>85</v>
+      </c>
+      <c r="D79">
+        <f>E78</f>
+        <v>75</v>
+      </c>
+      <c r="E79">
+        <f>D79-E68*E66</f>
+        <v>25</v>
+      </c>
+      <c r="F79">
+        <f>E66*E67</f>
+        <v>750000</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C80" t="s">
+        <v>538</v>
+      </c>
+      <c r="D80">
+        <f>E79</f>
+        <v>25</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <f>F67*D80/F68</f>
+        <v>225000</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F81">
+        <f>F80+F79+F78</f>
+        <v>1725000</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C82" t="s">
+        <v>540</v>
+      </c>
+      <c r="D82">
+        <f>F81</f>
+        <v>1725000</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B84">
+        <v>6.57</v>
+      </c>
+      <c r="D84" t="s">
+        <v>542</v>
+      </c>
+      <c r="E84" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C85" t="s">
+        <v>541</v>
+      </c>
+      <c r="D85">
+        <v>50</v>
+      </c>
+      <c r="E85">
+        <v>75</v>
+      </c>
+      <c r="F85">
+        <f>E85+D85</f>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C86" t="s">
+        <v>544</v>
+      </c>
+      <c r="D86">
+        <v>7.95</v>
+      </c>
+      <c r="E86">
+        <v>9.9499999999999993</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C87" t="s">
+        <v>545</v>
+      </c>
+      <c r="D87">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C88" t="s">
+        <v>546</v>
+      </c>
+      <c r="D88">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C90" t="s">
+        <v>547</v>
+      </c>
+      <c r="D90">
+        <v>100</v>
+      </c>
+      <c r="E90">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B92" t="s">
+        <v>7</v>
+      </c>
+      <c r="C92" t="s">
+        <v>548</v>
+      </c>
+      <c r="D92">
+        <f>D87+D88</f>
+        <v>850</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B94" t="s">
+        <v>9</v>
+      </c>
+      <c r="C94" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B96">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C97" t="s">
+        <v>550</v>
+      </c>
+      <c r="D97">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C98" t="s">
+        <v>551</v>
+      </c>
+      <c r="D98">
+        <v>1250000</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C99" t="s">
+        <v>552</v>
+      </c>
+      <c r="D99">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C100" t="s">
+        <v>553</v>
+      </c>
+      <c r="D100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C102" t="s">
+        <v>554</v>
+      </c>
+      <c r="D102">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C103" t="s">
+        <v>555</v>
+      </c>
+      <c r="D103">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C104" t="s">
+        <v>553</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C106" t="s">
+        <v>556</v>
+      </c>
+      <c r="D106">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B108" t="s">
+        <v>7</v>
+      </c>
+      <c r="C108" t="s">
+        <v>557</v>
+      </c>
+      <c r="D108">
+        <f>D102*D97*D99*D100-D103*D99+D106*D99</f>
+        <v>375000</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B110" t="s">
+        <v>9</v>
+      </c>
+      <c r="C110" t="s">
+        <v>558</v>
       </c>
     </row>
   </sheetData>
@@ -1888,8 +4011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA550D1-BAB1-4F6B-AEAA-D91F35147040}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2214,13 +4337,17 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD0019C-C6F8-4320-815D-EFECFFAEBA6B}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J113"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="G107" sqref="G107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="20.6328125" customWidth="1"/>
+    <col min="4" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -2432,10 +4559,19 @@
         <v>-1000</v>
       </c>
     </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="D25">
+        <f>SUM(D21:D24)</f>
+        <v>1225</v>
+      </c>
+    </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B26">
         <v>8.36</v>
       </c>
+      <c r="H26" t="s">
+        <v>559</v>
+      </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C27" t="s">
@@ -2514,7 +4650,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="E33" t="s">
+        <v>560</v>
+      </c>
+      <c r="F33" t="s">
+        <v>561</v>
+      </c>
+      <c r="G33" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
       <c r="C34" t="s">
         <v>152</v>
       </c>
@@ -2522,8 +4672,20 @@
         <f>(E27-F31)*D31</f>
         <v>-32.500000000000028</v>
       </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="E34">
+        <f>E30*E27</f>
+        <v>750</v>
+      </c>
+      <c r="F34">
+        <f>E27*D31</f>
+        <v>812.5</v>
+      </c>
+      <c r="G34">
+        <f>E31</f>
+        <v>845</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C35" t="s">
         <v>153</v>
       </c>
@@ -2532,7 +4694,10 @@
         <v>-62.5</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>9</v>
+      </c>
       <c r="C36" t="s">
         <v>154</v>
       </c>
@@ -2540,8 +4705,20 @@
         <f>(E28-F32)*D32</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="E36">
+        <f>F30*F32</f>
+        <v>6750</v>
+      </c>
+      <c r="F36">
+        <f>E32</f>
+        <v>7200</v>
+      </c>
+      <c r="G36">
+        <f>E32</f>
+        <v>7200</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C37" t="s">
         <v>155</v>
       </c>
@@ -2550,12 +4727,12 @@
         <v>-450</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B39">
         <v>8.42</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C40" t="s">
         <v>156</v>
       </c>
@@ -2563,7 +4740,7 @@
         <v>3150</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C41" t="s">
         <v>157</v>
       </c>
@@ -2571,7 +4748,7 @@
         <v>-4500</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C42" t="s">
         <v>158</v>
       </c>
@@ -2579,7 +4756,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C43" t="s">
         <v>159</v>
       </c>
@@ -2587,22 +4764,543 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="E44" t="s">
+        <v>560</v>
+      </c>
+      <c r="F44" t="s">
+        <v>561</v>
+      </c>
+      <c r="G44" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C45" t="s">
         <v>151</v>
       </c>
       <c r="D45">
-        <f>D41/D43+D42</f>
+        <f>F45/D43</f>
         <v>15000</v>
       </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="E45">
+        <f>D42*D43</f>
+        <v>27000</v>
+      </c>
+      <c r="F45">
+        <f>E45+D41</f>
+        <v>22500</v>
+      </c>
+      <c r="G45">
+        <f>F45+D40</f>
+        <v>25650</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C46" t="s">
         <v>160</v>
       </c>
       <c r="D46">
-        <f>D40/D45+D43</f>
+        <f>G45/D45</f>
         <v>1.71</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B48">
+        <v>8.5500000000000007</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C49" t="s">
+        <v>563</v>
+      </c>
+      <c r="D49">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C50" t="s">
+        <v>564</v>
+      </c>
+      <c r="D50">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C51" t="s">
+        <v>565</v>
+      </c>
+      <c r="D51">
+        <v>52500</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C52" t="s">
+        <v>566</v>
+      </c>
+      <c r="D52">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C53" t="s">
+        <v>567</v>
+      </c>
+      <c r="D53">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C54" t="s">
+        <v>568</v>
+      </c>
+      <c r="D54">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C56" t="s">
+        <v>569</v>
+      </c>
+      <c r="D56">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C57" t="s">
+        <v>156</v>
+      </c>
+      <c r="D57">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C58" t="s">
+        <v>157</v>
+      </c>
+      <c r="D58">
+        <v>-1875</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C59" t="s">
+        <v>570</v>
+      </c>
+      <c r="D59">
+        <v>-188</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C60" t="s">
+        <v>571</v>
+      </c>
+      <c r="D60">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B62" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" t="s">
+        <v>560</v>
+      </c>
+      <c r="F62" t="s">
+        <v>561</v>
+      </c>
+      <c r="G62" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C63" t="s">
+        <v>572</v>
+      </c>
+      <c r="D63">
+        <f>E63-D58/D52</f>
+        <v>150000000</v>
+      </c>
+      <c r="E63">
+        <f>D56*D51</f>
+        <v>131250000</v>
+      </c>
+      <c r="F63">
+        <f>G63-D57</f>
+        <v>149997000</v>
+      </c>
+      <c r="G63">
+        <f>D63</f>
+        <v>150000000</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B65" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C66" t="s">
+        <v>573</v>
+      </c>
+      <c r="D66">
+        <f>D52-D57/D63</f>
+        <v>8.0000000000000007E-5</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B68" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C69" t="s">
+        <v>574</v>
+      </c>
+      <c r="D69">
+        <f>-D60/D54+D56*D53/60</f>
+        <v>235</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B71" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C72" t="s">
+        <v>575</v>
+      </c>
+      <c r="D72">
+        <f>D54-D59/D69</f>
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B74">
+        <v>8.56</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C75" t="s">
+        <v>576</v>
+      </c>
+      <c r="D75">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C76" t="s">
+        <v>577</v>
+      </c>
+      <c r="D76">
+        <v>-2000</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C77" t="s">
+        <v>157</v>
+      </c>
+      <c r="D77">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C78" t="s">
+        <v>578</v>
+      </c>
+      <c r="D78">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C79" t="s">
+        <v>570</v>
+      </c>
+      <c r="D79">
+        <f>-500</f>
+        <v>-500</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C80" t="s">
+        <v>145</v>
+      </c>
+      <c r="D80">
+        <v>-4000</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C81" t="s">
+        <v>156</v>
+      </c>
+      <c r="D81">
+        <v>-1500</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C82" t="s">
+        <v>579</v>
+      </c>
+      <c r="D82">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F83" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B84" t="s">
+        <v>7</v>
+      </c>
+      <c r="C84" t="s">
+        <v>580</v>
+      </c>
+      <c r="D84">
+        <f>D75-D78</f>
+        <v>95000</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B86" t="s">
+        <v>9</v>
+      </c>
+      <c r="C86" t="s">
+        <v>144</v>
+      </c>
+      <c r="D86">
+        <f>D78-D80-D82-D76</f>
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B88" t="s">
+        <v>11</v>
+      </c>
+      <c r="C88" t="s">
+        <v>581</v>
+      </c>
+      <c r="D88">
+        <f>D86+D84</f>
+        <v>102000</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B90" t="s">
+        <v>12</v>
+      </c>
+      <c r="C90" t="s">
+        <v>571</v>
+      </c>
+      <c r="D90">
+        <f>D82-D81-D77-D79</f>
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B92">
+        <v>8.66</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C93" t="s">
+        <v>583</v>
+      </c>
+      <c r="D93">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C94" t="s">
+        <v>584</v>
+      </c>
+      <c r="D94">
+        <f>D93*2</f>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C96" s="4" t="s">
+        <v>585</v>
+      </c>
+      <c r="D96" t="s">
+        <v>586</v>
+      </c>
+      <c r="E96" t="s">
+        <v>589</v>
+      </c>
+      <c r="F96" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C97" s="4">
+        <v>45879</v>
+      </c>
+      <c r="D97" t="s">
+        <v>588</v>
+      </c>
+      <c r="E97">
+        <v>1000</v>
+      </c>
+      <c r="F97">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C98" s="4">
+        <v>45884</v>
+      </c>
+      <c r="D98" t="s">
+        <v>590</v>
+      </c>
+      <c r="E98">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C99" s="4">
+        <v>45891</v>
+      </c>
+      <c r="D99" t="s">
+        <v>588</v>
+      </c>
+      <c r="E99">
+        <v>800</v>
+      </c>
+      <c r="F99">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C100" s="4">
+        <v>45898</v>
+      </c>
+      <c r="D100" t="s">
+        <v>591</v>
+      </c>
+      <c r="E100">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B102" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102" t="s">
+        <v>592</v>
+      </c>
+      <c r="D102">
+        <f>D93+E97-E98+E99-E100</f>
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C103" t="s">
+        <v>593</v>
+      </c>
+      <c r="D103">
+        <f>D102*2</f>
+        <v>5600</v>
+      </c>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C104" t="s">
+        <v>594</v>
+      </c>
+      <c r="D104">
+        <f>(E98+E100)*2</f>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="106" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B106" t="s">
+        <v>9</v>
+      </c>
+      <c r="C106" t="s">
+        <v>595</v>
+      </c>
+      <c r="D106">
+        <f>(2-F97/E97)*E97+(2-F99/E99)*E99</f>
+        <v>-181.99999999999994</v>
+      </c>
+    </row>
+    <row r="108" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B108" t="s">
+        <v>11</v>
+      </c>
+      <c r="C108" t="s">
+        <v>596</v>
+      </c>
+      <c r="D108" t="s">
+        <v>597</v>
+      </c>
+      <c r="E108" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="109" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C109" t="s">
+        <v>598</v>
+      </c>
+      <c r="D109">
+        <f>D93</f>
+        <v>4000</v>
+      </c>
+      <c r="E109">
+        <f>D94</f>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="110" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C110" t="s">
+        <v>599</v>
+      </c>
+      <c r="D110">
+        <f>E97+E99</f>
+        <v>1800</v>
+      </c>
+      <c r="E110">
+        <f>F97+F99</f>
+        <v>3782</v>
+      </c>
+    </row>
+    <row r="111" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C111" t="s">
+        <v>600</v>
+      </c>
+      <c r="D111">
+        <f>E98+E100</f>
+        <v>3000</v>
+      </c>
+      <c r="E111">
+        <f>D111*2</f>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="112" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C112" t="s">
+        <v>601</v>
+      </c>
+      <c r="D112">
+        <v>0</v>
+      </c>
+      <c r="E112">
+        <v>-182</v>
+      </c>
+    </row>
+    <row r="113" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C113" t="s">
+        <v>602</v>
+      </c>
+      <c r="D113">
+        <f>D109+D110-D111+D112</f>
+        <v>2800</v>
+      </c>
+      <c r="E113">
+        <f>E109+E110-E111+E112</f>
+        <v>5600</v>
       </c>
     </row>
   </sheetData>
@@ -5120,7 +7818,7 @@
         <v>496500</v>
       </c>
       <c r="H20">
-        <f t="shared" ref="H18:H20" si="0">SUM(D20:G20)</f>
+        <f t="shared" ref="H20" si="0">SUM(D20:G20)</f>
         <v>973000</v>
       </c>
     </row>
@@ -5441,7 +8139,7 @@
         <v>395550</v>
       </c>
       <c r="H50">
-        <f t="shared" ref="H47:H57" si="5">SUM(D50:G50)</f>
+        <f t="shared" ref="H50:H57" si="5">SUM(D50:G50)</f>
         <v>708000</v>
       </c>
     </row>
@@ -5539,8 +8237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5854F927-407D-4435-A00B-79CB19DD567D}">
   <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6384,22 +9082,964 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83E35AA1-A86E-4AAE-ACC0-DDA3CDB3A684}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="24.54296875" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>15.32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>387</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>388</v>
+      </c>
+      <c r="D5">
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6">
+        <v>175000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>390</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>391</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>392</v>
+      </c>
+      <c r="D9">
+        <v>18750000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>393</v>
+      </c>
+      <c r="D10">
+        <v>7790000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
+        <v>394</v>
+      </c>
+      <c r="E12" t="s">
+        <v>335</v>
+      </c>
+      <c r="F12" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>397</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>398</v>
+      </c>
+      <c r="D15">
+        <f>D5+D6</f>
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>394</v>
+      </c>
+      <c r="D16">
+        <f>D15+D14</f>
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>400</v>
+      </c>
+      <c r="D18">
+        <f>D6</f>
+        <v>175000</v>
+      </c>
+      <c r="E18">
+        <f>D18</f>
+        <v>175000</v>
+      </c>
+      <c r="F18">
+        <f>D18</f>
+        <v>175000</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>401</v>
+      </c>
+      <c r="D19">
+        <f>D5</f>
+        <v>75000</v>
+      </c>
+      <c r="E19">
+        <f>D19*D7</f>
+        <v>75000</v>
+      </c>
+      <c r="F19">
+        <f>D19*D8</f>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>402</v>
+      </c>
+      <c r="D20">
+        <f>D19+D18</f>
+        <v>250000</v>
+      </c>
+      <c r="E20">
+        <f>E19+E18</f>
+        <v>250000</v>
+      </c>
+      <c r="F20">
+        <f>F19+F18</f>
+        <v>205000</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>404</v>
+      </c>
+      <c r="D22">
+        <f>E22+F22</f>
+        <v>26540000</v>
+      </c>
+      <c r="E22">
+        <f>D9</f>
+        <v>18750000</v>
+      </c>
+      <c r="F22">
+        <f>D10</f>
+        <v>7790000</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
+        <v>405</v>
+      </c>
+      <c r="D23">
+        <f>D22</f>
+        <v>26540000</v>
+      </c>
+      <c r="E23">
+        <f>E22</f>
+        <v>18750000</v>
+      </c>
+      <c r="F23">
+        <f>F22</f>
+        <v>7790000</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>407</v>
+      </c>
+      <c r="E25">
+        <f>E23/E20</f>
+        <v>75</v>
+      </c>
+      <c r="F25">
+        <f>F23/F20</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>409</v>
+      </c>
+      <c r="D27">
+        <f>E27+F27</f>
+        <v>19775000</v>
+      </c>
+      <c r="E27">
+        <f>E25*E18</f>
+        <v>13125000</v>
+      </c>
+      <c r="F27">
+        <f>F18*F25</f>
+        <v>6650000</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C28" t="s">
+        <v>410</v>
+      </c>
+      <c r="D28">
+        <f>E28+F28</f>
+        <v>6765000</v>
+      </c>
+      <c r="E28">
+        <f>E19*E25</f>
+        <v>5625000</v>
+      </c>
+      <c r="F28">
+        <f>F19*F25</f>
+        <v>1140000</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C29" t="s">
+        <v>411</v>
+      </c>
+      <c r="D29">
+        <f>E29+F29</f>
+        <v>26540000</v>
+      </c>
+      <c r="E29">
+        <f>E27+E28</f>
+        <v>18750000</v>
+      </c>
+      <c r="F29">
+        <f>F27+F28</f>
+        <v>7790000</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B31">
+        <v>15.33</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C32" t="s">
+        <v>412</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C33" t="s">
+        <v>413</v>
+      </c>
+      <c r="D33">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C34" t="s">
+        <v>414</v>
+      </c>
+      <c r="D34">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C35" t="s">
+        <v>415</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C36" t="s">
+        <v>416</v>
+      </c>
+      <c r="D36">
+        <v>3225000</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>417</v>
+      </c>
+      <c r="D38">
+        <f>D34</f>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" t="s">
+        <v>419</v>
+      </c>
+      <c r="D40">
+        <f>D33*D35</f>
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C41" t="s">
+        <v>418</v>
+      </c>
+      <c r="D41">
+        <f>D40+D38</f>
+        <v>107500</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" t="s">
+        <v>405</v>
+      </c>
+      <c r="D43">
+        <f>D36</f>
+        <v>3225000</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" t="s">
+        <v>407</v>
+      </c>
+      <c r="D45">
+        <f>D43/D41</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" t="s">
+        <v>420</v>
+      </c>
+      <c r="D47">
+        <f>D45*D38</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C48" t="s">
+        <v>421</v>
+      </c>
+      <c r="D48">
+        <f>D45*D40</f>
+        <v>225000</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C49" t="s">
+        <v>248</v>
+      </c>
+      <c r="D49">
+        <f>D48+D47</f>
+        <v>3225000</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B51">
+        <v>15.35</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C52" t="s">
+        <v>422</v>
+      </c>
+      <c r="D52" t="s">
+        <v>423</v>
+      </c>
+      <c r="E52" t="s">
+        <v>424</v>
+      </c>
+      <c r="F52" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C53" t="s">
+        <v>426</v>
+      </c>
+      <c r="D53">
+        <v>10000</v>
+      </c>
+      <c r="E53">
+        <v>7000</v>
+      </c>
+      <c r="F53">
+        <f>D57*D53+E57*E53</f>
+        <v>26400</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C54" t="s">
+        <v>427</v>
+      </c>
+      <c r="D54">
+        <v>90000</v>
+      </c>
+      <c r="E54">
+        <v>90000</v>
+      </c>
+      <c r="F54">
+        <v>270000</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C56" t="s">
+        <v>57</v>
+      </c>
+      <c r="D56">
+        <v>162000</v>
+      </c>
+      <c r="E56">
+        <v>108000</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C57" t="s">
+        <v>407</v>
+      </c>
+      <c r="D57">
+        <f>D56/D54</f>
+        <v>1.8</v>
+      </c>
+      <c r="E57">
+        <f>E56/E54</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B59">
+        <v>15.41</v>
+      </c>
+      <c r="E59" t="s">
+        <v>438</v>
+      </c>
+      <c r="F59" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C60" t="s">
+        <v>428</v>
+      </c>
+      <c r="D60" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C62" t="s">
+        <v>429</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C63" t="s">
+        <v>412</v>
+      </c>
+      <c r="D63">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C64" t="s">
+        <v>430</v>
+      </c>
+      <c r="D64">
+        <v>21200</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C65" t="s">
+        <v>431</v>
+      </c>
+      <c r="D65" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C66" t="s">
+        <v>432</v>
+      </c>
+      <c r="D66" s="3">
+        <v>1</v>
+      </c>
+      <c r="F66" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B67" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" t="s">
+        <v>433</v>
+      </c>
+      <c r="D67">
+        <v>10575000</v>
+      </c>
+      <c r="E67">
+        <f>D63</f>
+        <v>2300</v>
+      </c>
+      <c r="F67">
+        <f>E67+D$64</f>
+        <v>23500</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C68" t="s">
+        <v>434</v>
+      </c>
+      <c r="D68">
+        <v>58750000</v>
+      </c>
+      <c r="E68">
+        <f>D63</f>
+        <v>2300</v>
+      </c>
+      <c r="F68">
+        <f t="shared" ref="F68:F70" si="0">E68+D$64</f>
+        <v>23500</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C69" t="s">
+        <v>435</v>
+      </c>
+      <c r="D69">
+        <v>33525000</v>
+      </c>
+      <c r="E69">
+        <f>D63*D65</f>
+        <v>1150</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="0"/>
+        <v>22350</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C70" t="s">
+        <v>436</v>
+      </c>
+      <c r="D70">
+        <v>12720000</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="0"/>
+        <v>21200</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B72" t="s">
+        <v>9</v>
+      </c>
+      <c r="C72" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D73" t="s">
+        <v>248</v>
+      </c>
+      <c r="E73" t="s">
+        <v>433</v>
+      </c>
+      <c r="F73" t="s">
+        <v>434</v>
+      </c>
+      <c r="G73" t="s">
+        <v>435</v>
+      </c>
+      <c r="H73" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D74">
+        <f>SUM(E74:H74)</f>
+        <v>115570000</v>
+      </c>
+      <c r="E74">
+        <f>D67</f>
+        <v>10575000</v>
+      </c>
+      <c r="F74">
+        <f>D68</f>
+        <v>58750000</v>
+      </c>
+      <c r="G74">
+        <f>D69</f>
+        <v>33525000</v>
+      </c>
+      <c r="H74">
+        <f>D70</f>
+        <v>12720000</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C75" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D76">
+        <f>SUM(E76:H76)</f>
+        <v>5050</v>
+      </c>
+      <c r="E76">
+        <f>E74/F67</f>
+        <v>450</v>
+      </c>
+      <c r="F76">
+        <f>F74/F68</f>
+        <v>2500</v>
+      </c>
+      <c r="G76">
+        <f>G74/F69</f>
+        <v>1500</v>
+      </c>
+      <c r="H76">
+        <f>H74/F70</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C77" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C78" t="s">
+        <v>444</v>
+      </c>
+      <c r="D78">
+        <f>SUM(E78:H78)</f>
+        <v>107060000</v>
+      </c>
+      <c r="E78">
+        <f>E76*$D64</f>
+        <v>9540000</v>
+      </c>
+      <c r="F78">
+        <f t="shared" ref="F78:H78" si="1">F76*$D64</f>
+        <v>53000000</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="1"/>
+        <v>31800000</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="1"/>
+        <v>12720000</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C79" t="s">
+        <v>446</v>
+      </c>
+      <c r="D79">
+        <f>SUM(E79:H79)</f>
+        <v>8510000</v>
+      </c>
+      <c r="E79">
+        <f>E76*E67</f>
+        <v>1035000</v>
+      </c>
+      <c r="F79">
+        <f>F76*E68</f>
+        <v>5750000</v>
+      </c>
+      <c r="G79">
+        <f>G76*E69</f>
+        <v>1725000</v>
+      </c>
+      <c r="H79">
+        <f>E70*H76</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C80" t="s">
+        <v>248</v>
+      </c>
+      <c r="D80">
+        <f>D78+D79</f>
+        <v>115570000</v>
+      </c>
+      <c r="E80">
+        <f t="shared" ref="E80:H80" si="2">E78+E79</f>
+        <v>10575000</v>
+      </c>
+      <c r="F80">
+        <f t="shared" si="2"/>
+        <v>58750000</v>
+      </c>
+      <c r="G80">
+        <f t="shared" si="2"/>
+        <v>33525000</v>
+      </c>
+      <c r="H80">
+        <f t="shared" si="2"/>
+        <v>12720000</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B82">
+        <v>15.45</v>
+      </c>
+      <c r="D82" t="s">
+        <v>240</v>
+      </c>
+      <c r="E82" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C83" t="s">
+        <v>452</v>
+      </c>
+      <c r="D83" s="3">
+        <v>1</v>
+      </c>
+      <c r="E83" s="3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C84" t="s">
+        <v>453</v>
+      </c>
+      <c r="D84">
+        <v>330000</v>
+      </c>
+      <c r="E84">
+        <v>432000</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C85" t="s">
+        <v>454</v>
+      </c>
+      <c r="D85">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C86" t="s">
+        <v>455</v>
+      </c>
+      <c r="D86" s="3">
+        <v>1</v>
+      </c>
+      <c r="E86" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="F86">
+        <f>D84*D85/D94</f>
+        <v>300000</v>
+      </c>
+      <c r="G86">
+        <f>E84*E86*D94/(E83*D85)</f>
+        <v>633600</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C87" t="s">
+        <v>447</v>
+      </c>
+      <c r="D87">
+        <v>990000</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C88" t="s">
+        <v>448</v>
+      </c>
+      <c r="D88">
+        <v>2970000</v>
+      </c>
+      <c r="E88">
+        <v>1728000</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C89" t="s">
+        <v>449</v>
+      </c>
+      <c r="D89">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C90" t="s">
+        <v>451</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C91" t="s">
+        <v>95</v>
+      </c>
+      <c r="D91">
+        <v>800000</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C92" t="s">
+        <v>450</v>
+      </c>
+      <c r="D92">
+        <f>D89-D91</f>
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B94" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" t="s">
+        <v>456</v>
+      </c>
+      <c r="D94">
+        <f>D85+D89-D87</f>
+        <v>110000</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B96" t="s">
+        <v>9</v>
+      </c>
+      <c r="C96" t="s">
+        <v>457</v>
+      </c>
+      <c r="D96">
+        <f>D89+D85*E86-D94*E83</f>
+        <v>1014000</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B98" t="s">
+        <v>11</v>
+      </c>
+      <c r="C98" t="s">
+        <v>457</v>
+      </c>
+      <c r="D98">
+        <f>(D89+D86*D85-D83*D94)</f>
+        <v>990000</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C99" t="s">
+        <v>458</v>
+      </c>
+      <c r="D99">
+        <f>(D88+D84-F86)/D98</f>
+        <v>3.0303030303030303</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F100" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B101" t="s">
+        <v>12</v>
+      </c>
+      <c r="C101" t="s">
+        <v>455</v>
+      </c>
+      <c r="D101">
+        <f>D85*D99</f>
+        <v>303030.30303030304</v>
+      </c>
+      <c r="E101">
+        <f>D85*E86*(E84+E88)/D96</f>
+        <v>170414.20118343196</v>
+      </c>
+      <c r="F101">
+        <f>E101+D101</f>
+        <v>473444.504213735</v>
       </c>
     </row>
   </sheetData>

</xml_diff>